<commit_message>
add convert JFrame to image
</commit_message>
<xml_diff>
--- a/Result.xlsx
+++ b/Result.xlsx
@@ -20,6 +20,9 @@
     <t>119.3</t>
   </si>
   <si>
+    <t>47.3</t>
+  </si>
+  <si>
     <t>56.4</t>
   </si>
   <si>
@@ -41,31 +44,28 @@
     <t>12.9</t>
   </si>
   <si>
+    <t>21.1</t>
+  </si>
+  <si>
+    <t>94.7</t>
+  </si>
+  <si>
+    <t>69.8</t>
+  </si>
+  <si>
+    <t>42.1</t>
+  </si>
+  <si>
+    <t>83.5</t>
+  </si>
+  <si>
+    <t>32.4</t>
+  </si>
+  <si>
     <t>166.2</t>
   </si>
   <si>
-    <t>21.1</t>
-  </si>
-  <si>
-    <t>94.7</t>
-  </si>
-  <si>
-    <t>69.8</t>
-  </si>
-  <si>
-    <t>42.1</t>
-  </si>
-  <si>
-    <t>83.5</t>
-  </si>
-  <si>
-    <t>32.4</t>
-  </si>
-  <si>
     <t>66.4</t>
-  </si>
-  <si>
-    <t>47.3</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
add pain normal data and download gis to JPG
</commit_message>
<xml_diff>
--- a/Result.xlsx
+++ b/Result.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>91.9</t>
   </si>
@@ -27,9 +27,6 @@
   </si>
   <si>
     <t>50.2</t>
-  </si>
-  <si>
-    <t>0.0</t>
   </si>
   <si>
     <t>94.7</t>
@@ -98,7 +95,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:A18"/>
+  <dimension ref="A1:A13"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -136,62 +133,37 @@
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="0">
-        <v>5</v>
+        <v>9</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s" s="0">
-        <v>6</v>
+        <v>10</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s" s="0">
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s" s="0">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="s" s="0">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="s" s="0">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="s" s="0">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="s" s="0">
         <v>12</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="s" s="0">
-        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>